<commit_message>
Added tests to read extractor and css selectors realty attributes
</commit_message>
<xml_diff>
--- a/tests/files/config.xlsx
+++ b/tests/files/config.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Projects\sniffhome\tests\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255A13D7-4508-4C44-8A9F-CFFB89423764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B508F940-1D0D-465E-8B3A-92C1CD5C87DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{9BD48211-F718-4A97-9819-EE9DE14B1ADA}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{9BD48211-F718-4A97-9819-EE9DE14B1ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
     <sheet name="search_link" sheetId="4" r:id="rId2"/>
     <sheet name="list_schema" sheetId="2" r:id="rId3"/>
     <sheet name="attributes" sheetId="3" r:id="rId4"/>
+    <sheet name="extractor" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>COD</t>
   </si>
@@ -95,15 +96,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Neighborhood</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
@@ -174,14 +166,94 @@
   </si>
   <si>
     <t>test[change="get"]</t>
+  </si>
+  <si>
+    <t>a.publisher__name</t>
+  </si>
+  <si>
+    <t>.price__price-info</t>
+  </si>
+  <si>
+    <t>h1.title__title</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>p.title__address</t>
+  </si>
+  <si>
+    <t>li.features__item--bedroom</t>
+  </si>
+  <si>
+    <t>li.features__item--parking</t>
+  </si>
+  <si>
+    <t>Price Regex</t>
+  </si>
+  <si>
+    <t>Real State Regex</t>
+  </si>
+  <si>
+    <t>Condominium Regex</t>
+  </si>
+  <si>
+    <t>Other Tax Regex</t>
+  </si>
+  <si>
+    <t>Description Regex</t>
+  </si>
+  <si>
+    <t>Area Regex</t>
+  </si>
+  <si>
+    <t>Rooms Regex</t>
+  </si>
+  <si>
+    <t>Garage Regex</t>
+  </si>
+  <si>
+    <t>Neighborhood Regex</t>
+  </si>
+  <si>
+    <t>Street Regex</t>
+  </si>
+  <si>
+    <t>Supplier Code</t>
+  </si>
+  <si>
+    <t>span.condominium</t>
+  </si>
+  <si>
+    <t>span.iptu</t>
+  </si>
+  <si>
+    <t>SPLIT&lt;&gt;,&lt;&gt;1</t>
+  </si>
+  <si>
+    <t>REGEX&lt;&gt;\d+\.?\d*</t>
+  </si>
+  <si>
+    <t>REGEX&lt;&gt;\d+</t>
+  </si>
+  <si>
+    <t>SPLIT&lt;&gt;,&lt;&gt;0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -209,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -217,6 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,16 +618,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -565,13 +638,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -582,13 +655,13 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -599,7 +672,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -610,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -648,7 +721,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>14</v>
@@ -671,10 +744,10 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -682,19 +755,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E2" s="2">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -736,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE3E1B7-1FAE-4CD3-A5B8-25456555CB18}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,10 +836,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -788,67 +861,207 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF315C48-17B1-41F7-A267-478466903AFB}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
       </c>
       <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C90A6E1A-3F39-445D-B67B-5A698962F749}">
+          <x14:formula1>
+            <xm:f>meta!$A$3:$A$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5D249A-97DD-4084-86BB-D31D9EF1A754}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EBE25155-C9E9-4D32-B6CF-77F3F367AE70}">
+          <x14:formula1>
+            <xm:f>meta!$A$2:$A$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A40</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>